<commit_message>
added total value and average price
</commit_message>
<xml_diff>
--- a/trading_data.xlsx
+++ b/trading_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,36 +489,218 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>08/14/20</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>100</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-300000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3000</v>
+      </c>
+      <c r="H2" t="n">
+        <v>300000</v>
+      </c>
+      <c r="I2" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>08/14/20</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>200</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-600000</v>
+      </c>
+      <c r="G3" t="n">
+        <v>6000</v>
+      </c>
+      <c r="H3" t="n">
+        <v>900000</v>
+      </c>
+      <c r="I3" t="n">
+        <v>150</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>08/14/20</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>500</v>
+      </c>
+      <c r="E4" t="n">
+        <v>6000</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3000000</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
+        <v>150</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>CODX</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>12/12/12</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>08/14/20</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>BUY</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>30.49</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>400</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>-12196.00</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="D5" t="n">
+        <v>300</v>
+      </c>
+      <c r="E5" t="n">
+        <v>100</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-30000</v>
+      </c>
+      <c r="G5" t="n">
+        <v>100</v>
+      </c>
+      <c r="H5" t="n">
+        <v>30000</v>
+      </c>
+      <c r="I5" t="n">
+        <v>300</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>CODX</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>08/14/20</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>23.32</v>
+      </c>
+      <c r="E6" t="n">
+        <v>12999</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-303136.68</v>
+      </c>
+      <c r="G6" t="n">
+        <v>13099</v>
+      </c>
+      <c r="H6" t="n">
+        <v>333136.68</v>
+      </c>
+      <c r="I6" t="n">
+        <v>25.43</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CODX</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>08/14/20</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>300</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3000</v>
+      </c>
+      <c r="F7" t="n">
+        <v>900000</v>
+      </c>
+      <c r="G7" t="n">
+        <v>10099</v>
+      </c>
+      <c r="H7" t="n">
+        <v>256846.68</v>
+      </c>
+      <c r="I7" t="n">
+        <v>25.43</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
added comments, improved interaction
</commit_message>
<xml_diff>
--- a/trading_data.xlsx
+++ b/trading_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,6 +702,150 @@
       </c>
       <c r="J7" t="inlineStr"/>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>08/15/20</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>200</v>
+      </c>
+      <c r="E8" t="n">
+        <v>20</v>
+      </c>
+      <c r="F8" t="n">
+        <v>4000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>20</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4000</v>
+      </c>
+      <c r="I8" t="n">
+        <v>200</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>12/12/12</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>200</v>
+      </c>
+      <c r="E9" t="n">
+        <v>200</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-40000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>220</v>
+      </c>
+      <c r="H9" t="n">
+        <v>44000</v>
+      </c>
+      <c r="I9" t="n">
+        <v>200</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>08/15/20</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>12</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-156</v>
+      </c>
+      <c r="G10" t="n">
+        <v>233</v>
+      </c>
+      <c r="H10" t="n">
+        <v>44156</v>
+      </c>
+      <c r="I10" t="n">
+        <v>189.51</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>08/15/20</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>12</v>
+      </c>
+      <c r="E11" t="n">
+        <v>12</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-144</v>
+      </c>
+      <c r="G11" t="n">
+        <v>12</v>
+      </c>
+      <c r="H11" t="n">
+        <v>144</v>
+      </c>
+      <c r="I11" t="n">
+        <v>12</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
realized profit first implementation
Fixed bug where average_price was non-zero when we had 0 shares holding (after sell all for instance)

Implemented realized profit calculations
</commit_message>
<xml_diff>
--- a/trading_data.xlsx
+++ b/trading_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -846,6 +846,116 @@
       </c>
       <c r="J11" t="inlineStr"/>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>A</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>08/17/20</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>13</v>
+      </c>
+      <c r="E12" t="n">
+        <v>12</v>
+      </c>
+      <c r="F12" t="n">
+        <v>156</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>08/17/20</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>13</v>
+      </c>
+      <c r="E13" t="n">
+        <v>22</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-286</v>
+      </c>
+      <c r="G13" t="n">
+        <v>22</v>
+      </c>
+      <c r="H13" t="n">
+        <v>286</v>
+      </c>
+      <c r="I13" t="n">
+        <v>13</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>08/17/20</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>14</v>
+      </c>
+      <c r="E14" t="n">
+        <v>22</v>
+      </c>
+      <c r="F14" t="n">
+        <v>308</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
first implementation of iwe
</commit_message>
<xml_diff>
--- a/trading_data.xlsx
+++ b/trading_data.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -956,6 +956,42 @@
         <v>22</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>V</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>08/19/20</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>BUY</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>12</v>
+      </c>
+      <c r="E15" t="n">
+        <v>32</v>
+      </c>
+      <c r="F15" t="n">
+        <v>-384</v>
+      </c>
+      <c r="G15" t="n">
+        <v>32</v>
+      </c>
+      <c r="H15" t="n">
+        <v>384</v>
+      </c>
+      <c r="I15" t="n">
+        <v>12</v>
+      </c>
+      <c r="J15" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>